<commit_message>
Chart + Table for WCAG Counts Completed
</commit_message>
<xml_diff>
--- a/original.xlsx
+++ b/original.xlsx
@@ -24,6 +24,7 @@
     <sheet name="Notifications" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="View Statement" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="Statement Preference" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Trying" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
@@ -3420,6 +3421,118 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>WCAG 2.1 AA Success Criteria Distribution</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Trying'!B2</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Trying'!$A$3:$A$29</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Trying'!$B$3:$B$29</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>WCAG Success Criteria #</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Defect Count</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
@@ -3558,6 +3671,44 @@
     <clientData/>
   </twoCellAnchor>
 </wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>9</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9720000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="WCAG_Counts" displayName="WCAG_Counts" ref="A2:B29" headerRowCount="1">
+  <autoFilter ref="A2:B29"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="WCAG_SC"/>
+    <tableColumn id="2" name="No_of_occurence"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3861,7 +4012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:I130"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:C30"/>
@@ -3873,6 +4024,7 @@
     <col width="11.140625" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2" ht="17.25" customHeight="1">
       <c r="B2" s="6" t="inlineStr">
         <is>
@@ -3880,6 +4032,7 @@
         </is>
       </c>
     </row>
+    <row r="3"/>
     <row r="4">
       <c r="B4" s="1" t="inlineStr">
         <is>
@@ -4152,6 +4305,8 @@
         <v>10</v>
       </c>
     </row>
+    <row r="31"/>
+    <row r="32"/>
     <row r="33" ht="17.25" customHeight="1">
       <c r="B33" s="6" t="inlineStr">
         <is>
@@ -4159,6 +4314,7 @@
         </is>
       </c>
     </row>
+    <row r="34"/>
     <row r="35">
       <c r="B35" s="1" t="n"/>
       <c r="C35" s="1" t="inlineStr">
@@ -4201,6 +4357,17 @@
         <v>127</v>
       </c>
     </row>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
     <row r="48" ht="17.25" customHeight="1">
       <c r="B48" s="6" t="inlineStr">
         <is>
@@ -4241,6 +4408,16 @@
         <v>87</v>
       </c>
     </row>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
     <row r="62">
       <c r="B62" t="inlineStr">
         <is>
@@ -4315,6 +4492,15 @@
         <v>19</v>
       </c>
     </row>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
     <row r="75" ht="17.25" customHeight="1">
       <c r="B75" s="6" t="inlineStr">
         <is>
@@ -4322,6 +4508,7 @@
         </is>
       </c>
     </row>
+    <row r="76"/>
     <row r="77">
       <c r="B77" t="inlineStr">
         <is>
@@ -4355,6 +4542,7 @@
         <v>14</v>
       </c>
     </row>
+    <row r="79"/>
     <row r="80">
       <c r="B80" t="inlineStr">
         <is>
@@ -14081,13 +14269,329 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>WCAG Rule Wise Defect Distribution Chart</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="170" t="inlineStr">
+        <is>
+          <t>WCAG_SC</t>
+        </is>
+      </c>
+      <c r="B2" s="170" t="inlineStr">
+        <is>
+          <t>No_of_occurence</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="171" t="inlineStr">
+        <is>
+          <t>1.1.1 Non Text Content</t>
+        </is>
+      </c>
+      <c r="B3" s="171" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="171" t="inlineStr">
+        <is>
+          <t>1.3.1 Info and Relationship</t>
+        </is>
+      </c>
+      <c r="B4" s="171" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="171" t="inlineStr">
+        <is>
+          <t>1.3.2 Meaningful Sequence</t>
+        </is>
+      </c>
+      <c r="B5" s="171" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="171" t="inlineStr">
+        <is>
+          <t>1.3.4 Orientation</t>
+        </is>
+      </c>
+      <c r="B6" s="171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="171" t="inlineStr">
+        <is>
+          <t>1.3.5 Identify Input Purpose</t>
+        </is>
+      </c>
+      <c r="B7" s="171" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="171" t="inlineStr">
+        <is>
+          <t>1.4.1 Use of Color</t>
+        </is>
+      </c>
+      <c r="B8" s="171" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="171" t="inlineStr">
+        <is>
+          <t>1.4.3 Contrast (Minimum)</t>
+        </is>
+      </c>
+      <c r="B9" s="171" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="171" t="inlineStr">
+        <is>
+          <t>1.4.4 Resize Text</t>
+        </is>
+      </c>
+      <c r="B10" s="171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="171" t="inlineStr">
+        <is>
+          <t>1.4.5 Image of Text</t>
+        </is>
+      </c>
+      <c r="B11" s="171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="171" t="inlineStr">
+        <is>
+          <t>1.4.10 Reflow</t>
+        </is>
+      </c>
+      <c r="B12" s="171" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="171" t="inlineStr">
+        <is>
+          <t>1.4.11 Non Text Contrast</t>
+        </is>
+      </c>
+      <c r="B13" s="171" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="171" t="inlineStr">
+        <is>
+          <t>1.4.12 Text Spacing</t>
+        </is>
+      </c>
+      <c r="B14" s="171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="171" t="inlineStr">
+        <is>
+          <t>2.1.1 Keyboard</t>
+        </is>
+      </c>
+      <c r="B15" s="171" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="171" t="inlineStr">
+        <is>
+          <t>2.1.2 No Keyboard Trap</t>
+        </is>
+      </c>
+      <c r="B16" s="171" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="171" t="inlineStr">
+        <is>
+          <t>2.2.1 Timing Adjustable</t>
+        </is>
+      </c>
+      <c r="B17" s="171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="171" t="inlineStr">
+        <is>
+          <t>2.4.2 Page Titled</t>
+        </is>
+      </c>
+      <c r="B18" s="171" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="171" t="inlineStr">
+        <is>
+          <t>2.4.3 Focus Order</t>
+        </is>
+      </c>
+      <c r="B19" s="171" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="171" t="inlineStr">
+        <is>
+          <t>2.4.4 Link Purpose (In Context)</t>
+        </is>
+      </c>
+      <c r="B20" s="171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="171" t="inlineStr">
+        <is>
+          <t>2.4.6 Headings and Labels</t>
+        </is>
+      </c>
+      <c r="B21" s="171" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="171" t="inlineStr">
+        <is>
+          <t>2.4.7 Focus Visible</t>
+        </is>
+      </c>
+      <c r="B22" s="171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="171" t="inlineStr">
+        <is>
+          <t>3.1.1 Language of Page</t>
+        </is>
+      </c>
+      <c r="B23" s="171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="171" t="inlineStr">
+        <is>
+          <t>3.2.2 On Input</t>
+        </is>
+      </c>
+      <c r="B24" s="171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="171" t="inlineStr">
+        <is>
+          <t>3.3.2 Label or Instructions</t>
+        </is>
+      </c>
+      <c r="B25" s="171" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="171" t="inlineStr">
+        <is>
+          <t>3.3.3 Error Suggestion</t>
+        </is>
+      </c>
+      <c r="B26" s="171" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="171" t="inlineStr">
+        <is>
+          <t>4.1.1 Parsing</t>
+        </is>
+      </c>
+      <c r="B27" s="171" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="171" t="inlineStr">
+        <is>
+          <t>4.1.2 Name, Role, Value</t>
+        </is>
+      </c>
+      <c r="B28" s="171" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="171" t="inlineStr">
+        <is>
+          <t>4.1.3 Status Message</t>
+        </is>
+      </c>
+      <c r="B29" s="171" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C15" sqref="C15:C16"/>
@@ -14165,6 +14669,7 @@
       <c r="B12" s="8" t="n"/>
       <c r="C12" s="159" t="n"/>
     </row>
+    <row r="13"/>
     <row r="14" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="15">
       <c r="B15" s="143" t="inlineStr">
@@ -14302,7 +14807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:XEW18"/>
+  <dimension ref="A1:XEW18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>

</xml_diff>

<commit_message>
Fixed the Lables for Chart
</commit_message>
<xml_diff>
--- a/original.xlsx
+++ b/original.xlsx
@@ -3467,6 +3467,12 @@
             </numRef>
           </val>
         </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+        </dLbls>
         <gapWidth val="150"/>
         <axId val="10"/>
         <axId val="100"/>

</xml_diff>

<commit_message>
Severity and Counts Table + Chart Working code
</commit_message>
<xml_diff>
--- a/original.xlsx
+++ b/original.xlsx
@@ -34,7 +34,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="14">
+  <fonts count="19">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -115,6 +115,30 @@
     <font/>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <color rgb="000070C0"/>
+      <sz val="13"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="14"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="00B4C6E7"/>
+      <sz val="13"/>
+    </font>
+    <font>
+      <color rgb="FFB4C6E7"/>
+      <sz val="13"/>
+    </font>
+    <font>
+      <color rgb="002F5496"/>
+      <sz val="13"/>
     </font>
   </fonts>
   <fills count="13">
@@ -739,7 +763,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1212,6 +1236,21 @@
     <xf numFmtId="0" fontId="12" fillId="11" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3448,7 +3487,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Trying'!B2</f>
+              <f>'Trying'!C4</f>
             </strRef>
           </tx>
           <spPr>
@@ -3458,12 +3497,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Trying'!$A$3:$A$29</f>
+              <f>'Trying'!$B$5:$B$31</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Trying'!$B$3:$B$29</f>
+              <f>'Trying'!$C$5:$C$31</f>
             </numRef>
           </val>
         </ser>
@@ -3527,6 +3566,127 @@
         </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Severity/Impact Wise Defect Distribution</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Trying'!B37</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Trying'!$C$36:$F$36</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Trying'!$C$37:$F$37</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Defect Impact Category</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="in"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="low"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Defect Count</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="in"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="low"/>
         <crossAx val="10"/>
       </valAx>
     </plotArea>
@@ -3683,12 +3843,12 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>4</col>
+      <col>5</col>
       <colOff>0</colOff>
-      <row>9</row>
+      <row>8</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9720000" cy="3600000"/>
+    <ext cx="9000000" cy="3240000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -3703,15 +3863,51 @@
     </graphicFrame>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>33</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="WCAG_Counts" displayName="WCAG_Counts" ref="A2:B29" headerRowCount="1">
-  <autoFilter ref="A2:B29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="WCAG_Counts" displayName="WCAG_Counts" ref="B4:C31" headerRowCount="1">
+  <autoFilter ref="B4:C31"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="WCAG_SC"/>
-    <tableColumn id="2" name="No_of_occurence"/>
+    <tableColumn id="2" name="WCAG_SC"/>
+    <tableColumn id="3" name="No_of_occurence"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="DefectCountTable" displayName="DefectCountTable" ref="B36:F37" headerRowCount="1">
+  <autoFilter ref="B36:F37"/>
+  <tableColumns count="5">
+    <tableColumn id="2" name=""/>
+    <tableColumn id="3" name="Critical"/>
+    <tableColumn id="4" name="High"/>
+    <tableColumn id="5" name="Medium"/>
+    <tableColumn id="6" name="Low"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14281,7 +14477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A2:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14289,304 +14485,358 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="2">
+      <c r="B2" s="180" t="inlineStr">
         <is>
           <t>WCAG Rule Wise Defect Distribution Chart</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="170" t="inlineStr">
+    <row r="4">
+      <c r="B4" s="170" t="inlineStr">
         <is>
           <t>WCAG_SC</t>
         </is>
       </c>
-      <c r="B2" s="170" t="inlineStr">
+      <c r="C4" s="170" t="inlineStr">
         <is>
           <t>No_of_occurence</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="171" t="inlineStr">
+    <row r="5">
+      <c r="B5" s="171" t="inlineStr">
         <is>
           <t>1.1.1 Non Text Content</t>
         </is>
       </c>
-      <c r="B3" s="171" t="n">
+      <c r="C5" s="171" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="171" t="inlineStr">
+    <row r="6">
+      <c r="B6" s="171" t="inlineStr">
         <is>
           <t>1.3.1 Info and Relationship</t>
         </is>
       </c>
-      <c r="B4" s="171" t="n">
+      <c r="C6" s="171" t="n">
         <v>54</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="171" t="inlineStr">
+    <row r="7">
+      <c r="B7" s="171" t="inlineStr">
         <is>
           <t>1.3.2 Meaningful Sequence</t>
         </is>
       </c>
-      <c r="B5" s="171" t="n">
+      <c r="C7" s="171" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="171" t="inlineStr">
+    <row r="8">
+      <c r="B8" s="171" t="inlineStr">
         <is>
           <t>1.3.4 Orientation</t>
         </is>
       </c>
-      <c r="B6" s="171" t="n">
+      <c r="C8" s="171" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="171" t="inlineStr">
+    <row r="9">
+      <c r="B9" s="171" t="inlineStr">
         <is>
           <t>1.3.5 Identify Input Purpose</t>
         </is>
       </c>
-      <c r="B7" s="171" t="n">
+      <c r="C9" s="171" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="171" t="inlineStr">
+    <row r="10">
+      <c r="B10" s="171" t="inlineStr">
         <is>
           <t>1.4.1 Use of Color</t>
         </is>
       </c>
-      <c r="B8" s="171" t="n">
+      <c r="C10" s="171" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="171" t="inlineStr">
+    <row r="11">
+      <c r="B11" s="171" t="inlineStr">
         <is>
           <t>1.4.3 Contrast (Minimum)</t>
         </is>
       </c>
-      <c r="B9" s="171" t="n">
+      <c r="C11" s="171" t="n">
         <v>39</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="171" t="inlineStr">
+    <row r="12">
+      <c r="B12" s="171" t="inlineStr">
         <is>
           <t>1.4.4 Resize Text</t>
         </is>
       </c>
-      <c r="B10" s="171" t="n">
+      <c r="C12" s="171" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="171" t="inlineStr">
+    <row r="13">
+      <c r="B13" s="171" t="inlineStr">
         <is>
           <t>1.4.5 Image of Text</t>
         </is>
       </c>
-      <c r="B11" s="171" t="n">
+      <c r="C13" s="171" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="171" t="inlineStr">
+    <row r="14">
+      <c r="B14" s="171" t="inlineStr">
         <is>
           <t>1.4.10 Reflow</t>
         </is>
       </c>
-      <c r="B12" s="171" t="n">
+      <c r="C14" s="171" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="171" t="inlineStr">
+    <row r="15">
+      <c r="B15" s="171" t="inlineStr">
         <is>
           <t>1.4.11 Non Text Contrast</t>
         </is>
       </c>
-      <c r="B13" s="171" t="n">
+      <c r="C15" s="171" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="171" t="inlineStr">
+    <row r="16">
+      <c r="B16" s="171" t="inlineStr">
         <is>
           <t>1.4.12 Text Spacing</t>
         </is>
       </c>
-      <c r="B14" s="171" t="n">
+      <c r="C16" s="171" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="171" t="inlineStr">
+    <row r="17">
+      <c r="B17" s="171" t="inlineStr">
         <is>
           <t>2.1.1 Keyboard</t>
         </is>
       </c>
-      <c r="B15" s="171" t="n">
+      <c r="C17" s="171" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="171" t="inlineStr">
+    <row r="18">
+      <c r="B18" s="171" t="inlineStr">
         <is>
           <t>2.1.2 No Keyboard Trap</t>
         </is>
       </c>
-      <c r="B16" s="171" t="n">
+      <c r="C18" s="171" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="171" t="inlineStr">
+    <row r="19">
+      <c r="B19" s="171" t="inlineStr">
         <is>
           <t>2.2.1 Timing Adjustable</t>
         </is>
       </c>
-      <c r="B17" s="171" t="n">
+      <c r="C19" s="171" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="171" t="inlineStr">
+    <row r="20">
+      <c r="B20" s="171" t="inlineStr">
         <is>
           <t>2.4.2 Page Titled</t>
         </is>
       </c>
-      <c r="B18" s="171" t="n">
+      <c r="C20" s="171" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="171" t="inlineStr">
+    <row r="21">
+      <c r="B21" s="171" t="inlineStr">
         <is>
           <t>2.4.3 Focus Order</t>
         </is>
       </c>
-      <c r="B19" s="171" t="n">
+      <c r="C21" s="171" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="171" t="inlineStr">
+    <row r="22">
+      <c r="B22" s="171" t="inlineStr">
         <is>
           <t>2.4.4 Link Purpose (In Context)</t>
         </is>
       </c>
-      <c r="B20" s="171" t="n">
+      <c r="C22" s="171" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="171" t="inlineStr">
+    <row r="23">
+      <c r="B23" s="171" t="inlineStr">
         <is>
           <t>2.4.6 Headings and Labels</t>
         </is>
       </c>
-      <c r="B21" s="171" t="n">
+      <c r="C23" s="171" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="171" t="inlineStr">
+    <row r="24">
+      <c r="B24" s="171" t="inlineStr">
         <is>
           <t>2.4.7 Focus Visible</t>
         </is>
       </c>
-      <c r="B22" s="171" t="n">
+      <c r="C24" s="171" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="171" t="inlineStr">
+    <row r="25">
+      <c r="B25" s="171" t="inlineStr">
         <is>
           <t>3.1.1 Language of Page</t>
         </is>
       </c>
-      <c r="B23" s="171" t="n">
+      <c r="C25" s="171" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="171" t="inlineStr">
+    <row r="26">
+      <c r="B26" s="171" t="inlineStr">
         <is>
           <t>3.2.2 On Input</t>
         </is>
       </c>
-      <c r="B24" s="171" t="n">
+      <c r="C26" s="171" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="171" t="inlineStr">
+    <row r="27">
+      <c r="B27" s="171" t="inlineStr">
         <is>
           <t>3.3.2 Label or Instructions</t>
         </is>
       </c>
-      <c r="B25" s="171" t="n">
+      <c r="C27" s="171" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="171" t="inlineStr">
+    <row r="28">
+      <c r="B28" s="171" t="inlineStr">
         <is>
           <t>3.3.3 Error Suggestion</t>
         </is>
       </c>
-      <c r="B26" s="171" t="n">
+      <c r="C28" s="171" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="171" t="inlineStr">
+    <row r="29">
+      <c r="B29" s="171" t="inlineStr">
         <is>
           <t>4.1.1 Parsing</t>
         </is>
       </c>
-      <c r="B27" s="171" t="n">
+      <c r="C29" s="171" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="171" t="inlineStr">
+    <row r="30">
+      <c r="B30" s="171" t="inlineStr">
         <is>
           <t>4.1.2 Name, Role, Value</t>
         </is>
       </c>
-      <c r="B28" s="171" t="n">
+      <c r="C30" s="171" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="171" t="inlineStr">
+    <row r="31">
+      <c r="B31" s="171" t="inlineStr">
         <is>
           <t>4.1.3 Status Message</t>
         </is>
       </c>
-      <c r="B29" s="171" t="n">
+      <c r="C31" s="171" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" s="180" t="inlineStr">
+        <is>
+          <t>Severity/Impact Wise Defect Distribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" s="171" t="inlineStr"/>
+      <c r="C36" s="171" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="D36" s="171" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E36" s="171" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="F36" s="171" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" s="171" t="inlineStr">
+        <is>
+          <t>Defect count</t>
+        </is>
+      </c>
+      <c r="C37" s="171">
+        <f>SUM('Execution Summary'!O4:O200 )</f>
+        <v/>
+      </c>
+      <c r="D37" s="171">
+        <f>SUM('Execution Summary'!P4:P200 )</f>
+        <v/>
+      </c>
+      <c r="E37" s="171">
+        <f>SUM('Execution Summary'!Q4:Q200 )</f>
+        <v/>
+      </c>
+      <c r="F37" s="171">
+        <f>SUM('Execution Summary'!R4:R200 )</f>
+        <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Severity , Counts , Conformance Table and Chart Completed
</commit_message>
<xml_diff>
--- a/original.xlsx
+++ b/original.xlsx
@@ -3699,6 +3699,127 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Severity/Impact Wise Defect Distribution</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Trying'!B52</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Trying'!$C$51:$D$51</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Trying'!$C$52:$D$52</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Defect Impact Category</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="in"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="low"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Defect Count</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="in"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="low"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
@@ -3867,7 +3988,7 @@
     <from>
       <col>7</col>
       <colOff>0</colOff>
-      <row>33</row>
+      <row>32</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -3880,6 +4001,28 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>47</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3908,6 +4051,18 @@
     <tableColumn id="4" name="High"/>
     <tableColumn id="5" name="Medium"/>
     <tableColumn id="6" name="Low"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="ConformanceCountTable" displayName="ConformanceCountTable" ref="B51:D52" headerRowCount="1">
+  <autoFilter ref="B51:D52"/>
+  <tableColumns count="3">
+    <tableColumn id="2" name="Conformance Level"/>
+    <tableColumn id="3" name="A"/>
+    <tableColumn id="4" name="AA"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14477,7 +14632,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F37"/>
+  <dimension ref="A2:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14831,12 +14986,52 @@
         <v/>
       </c>
     </row>
+    <row r="49">
+      <c r="B49" s="180" t="inlineStr">
+        <is>
+          <t>Conformance Level Wise Defect Distribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" s="171" t="inlineStr">
+        <is>
+          <t>Conformance Level</t>
+        </is>
+      </c>
+      <c r="C51" s="171" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D51" s="171" t="inlineStr">
+        <is>
+          <t>AA</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" s="171" t="inlineStr">
+        <is>
+          <t>Defect count</t>
+        </is>
+      </c>
+      <c r="C52" s="171">
+        <f>SUM('Execution Summary'!F4:F200 )</f>
+        <v/>
+      </c>
+      <c r="D52" s="171">
+        <f>SUM('Execution Summary'!G4:G200 )</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Severity , Conformance , Issue Type , Counts Table + Chart Done
</commit_message>
<xml_diff>
--- a/original.xlsx
+++ b/original.xlsx
@@ -3771,7 +3771,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Defect Impact Category</a:t>
+                  <a:t>Conformance Level</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -3810,6 +3810,72 @@
         <tickLblPos val="low"/>
         <crossAx val="10"/>
       </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Severity/Impact Wise Defect Distribution</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Trying'!B67</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Trying'!$C$66:$I$66</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Trying'!$C$67:$I$67</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <dLblPos val="outEnd"/>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="1"/>
+          <showSerName val="0"/>
+          <showPercent val="1"/>
+          <showLeaderLines val="1"/>
+        </dLbls>
+        <firstSliceAng val="0"/>
+      </pieChart>
     </plotArea>
     <legend>
       <legendPos val="r"/>
@@ -4028,6 +4094,28 @@
     </graphicFrame>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>62</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5760000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -4063,6 +4151,23 @@
     <tableColumn id="2" name="Conformance Level"/>
     <tableColumn id="3" name="A"/>
     <tableColumn id="4" name="AA"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="IssuetypeCountTable" displayName="IssuetypeCountTable" ref="B66:I67" headerRowCount="1">
+  <autoFilter ref="B66:I67"/>
+  <tableColumns count="8">
+    <tableColumn id="2" name=""/>
+    <tableColumn id="3" name="Keyboard Navigation"/>
+    <tableColumn id="4" name="Color Contrast"/>
+    <tableColumn id="5" name="Color"/>
+    <tableColumn id="6" name="Zoom"/>
+    <tableColumn id="7" name="HTML Validator"/>
+    <tableColumn id="8" name="Screen Reader"/>
+    <tableColumn id="9" name="Other A11y"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14632,7 +14737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F52"/>
+  <dimension ref="A2:I67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15025,13 +15130,94 @@
         <v/>
       </c>
     </row>
+    <row r="64">
+      <c r="B64" s="180" t="inlineStr">
+        <is>
+          <t>Severity/Impact Wise Defect Distribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" s="171" t="inlineStr"/>
+      <c r="C66" s="171" t="inlineStr">
+        <is>
+          <t>Keyboard Navigation</t>
+        </is>
+      </c>
+      <c r="D66" s="171" t="inlineStr">
+        <is>
+          <t>Color Contrast</t>
+        </is>
+      </c>
+      <c r="E66" s="171" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="F66" s="171" t="inlineStr">
+        <is>
+          <t>Zoom</t>
+        </is>
+      </c>
+      <c r="G66" s="171" t="inlineStr">
+        <is>
+          <t>HTML Validator</t>
+        </is>
+      </c>
+      <c r="H66" s="171" t="inlineStr">
+        <is>
+          <t>Screen Reader</t>
+        </is>
+      </c>
+      <c r="I66" s="171" t="inlineStr">
+        <is>
+          <t>Other A11y</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" s="171" t="inlineStr">
+        <is>
+          <t>Defect count</t>
+        </is>
+      </c>
+      <c r="C67" s="171">
+        <f>SUM('Execution Summary'!H4:H200 )</f>
+        <v/>
+      </c>
+      <c r="D67" s="171">
+        <f>SUM('Execution Summary'!I4:I200 )</f>
+        <v/>
+      </c>
+      <c r="E67" s="171">
+        <f>SUM('Execution Summary'!J4:J200 )</f>
+        <v/>
+      </c>
+      <c r="F67" s="171">
+        <f>SUM('Execution Summary'!K4:K200 )</f>
+        <v/>
+      </c>
+      <c r="G67" s="171">
+        <f>SUM('Execution Summary'!L4:L200 )</f>
+        <v/>
+      </c>
+      <c r="H67" s="171">
+        <f>SUM('Execution Summary'!M4:M200 )</f>
+        <v/>
+      </c>
+      <c r="I67" s="171">
+        <f>SUM('Execution Summary'!N4:N200 )</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -15258,7 +15444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:XEW18"/>
+  <dimension ref="A1:XEW19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
@@ -16399,6 +16585,7 @@
         <v>6</v>
       </c>
     </row>
+    <row r="19"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="F2:G2"/>

</xml_diff>

<commit_message>
All charts and Tables Done
</commit_message>
<xml_diff>
--- a/original.xlsx
+++ b/original.xlsx
@@ -1937,6 +1937,72 @@
       <a:round/>
     </a:ln>
   </spPr>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Severity/Impact Wise Defect Distribution</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Trying'!B82</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Trying'!$C$81:$E$81</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Trying'!$C$82:$E$82</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <dLblPos val="outEnd"/>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="1"/>
+          <showSerName val="0"/>
+          <showPercent val="1"/>
+          <showLeaderLines val="1"/>
+        </dLbls>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
 </chartSpace>
 </file>
 
@@ -4116,6 +4182,28 @@
     </graphicFrame>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>83</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5760000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="5" name="Chart 5"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -4168,6 +4256,30 @@
     <tableColumn id="7" name="HTML Validator"/>
     <tableColumn id="8" name="Screen Reader"/>
     <tableColumn id="9" name="Other A11y"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Status_table" displayName="Status_table" ref="B88:C138" headerRowCount="1">
+  <autoFilter ref="B88:C138"/>
+  <tableColumns count="2">
+    <tableColumn id="2" name="WCAG_SC"/>
+    <tableColumn id="3" name="Result"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Status_counts_table" displayName="Status_counts_table" ref="B81:E82" headerRowCount="1">
+  <autoFilter ref="B81:E82"/>
+  <tableColumns count="4">
+    <tableColumn id="2" name="Result"/>
+    <tableColumn id="3" name="Fail"/>
+    <tableColumn id="4" name="Pass"/>
+    <tableColumn id="5" name="N/A"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14737,7 +14849,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:I67"/>
+  <dimension ref="A2:I138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15210,14 +15322,679 @@
         <v/>
       </c>
     </row>
+    <row r="79">
+      <c r="B79" s="180" t="inlineStr">
+        <is>
+          <t>Conformance Level Wise Defect Distribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" s="171" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="C81" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="D81" s="171" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E81" s="171" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" s="171" t="inlineStr"/>
+      <c r="C82" s="171">
+        <f>COUNTIF(C89:C138, "Fail")</f>
+        <v/>
+      </c>
+      <c r="D82" s="171">
+        <f>COUNTIF(C89:C138, "Pass")</f>
+        <v/>
+      </c>
+      <c r="E82" s="171">
+        <f>COUNTIF(C89:C138, "N/A")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" s="180" t="inlineStr">
+        <is>
+          <t>Severity/Impact Wise Defect Distribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" s="170" t="inlineStr">
+        <is>
+          <t>WCAG_SC</t>
+        </is>
+      </c>
+      <c r="C88" s="170" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" s="171" t="inlineStr">
+        <is>
+          <t>1.1.1 Non Text Content</t>
+        </is>
+      </c>
+      <c r="C89" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" s="171" t="inlineStr">
+        <is>
+          <t>1.2.1 Audio-only and Video-only (Prerecorded)</t>
+        </is>
+      </c>
+      <c r="C90" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" s="171" t="inlineStr">
+        <is>
+          <t>1.2.2 Captions</t>
+        </is>
+      </c>
+      <c r="C91" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" s="171" t="inlineStr">
+        <is>
+          <t>1.2.3 Audio Descriptions and Media Alternative (Prerecorded)</t>
+        </is>
+      </c>
+      <c r="C92" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" s="171" t="inlineStr">
+        <is>
+          <t>1.2.4 Captions (Live)</t>
+        </is>
+      </c>
+      <c r="C93" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" s="171" t="inlineStr">
+        <is>
+          <t>1.2.5 Audio Description (Prerecorded)</t>
+        </is>
+      </c>
+      <c r="C94" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" s="171" t="inlineStr">
+        <is>
+          <t>1.3.1 Info and Relationship</t>
+        </is>
+      </c>
+      <c r="C95" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" s="171" t="inlineStr">
+        <is>
+          <t>1.3.2 Meaningful Sequence</t>
+        </is>
+      </c>
+      <c r="C96" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" s="171" t="inlineStr">
+        <is>
+          <t>1.3.3 Sensory Characteristics</t>
+        </is>
+      </c>
+      <c r="C97" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" s="171" t="inlineStr">
+        <is>
+          <t>1.3.4 Orientation</t>
+        </is>
+      </c>
+      <c r="C98" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" s="171" t="inlineStr">
+        <is>
+          <t>1.3.5 Identify Input Purpose</t>
+        </is>
+      </c>
+      <c r="C99" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" s="171" t="inlineStr">
+        <is>
+          <t>1.4.1 Use of Color</t>
+        </is>
+      </c>
+      <c r="C100" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" s="171" t="inlineStr">
+        <is>
+          <t>1.4.2 Audio Control</t>
+        </is>
+      </c>
+      <c r="C101" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" s="171" t="inlineStr">
+        <is>
+          <t>1.4.3 Contrast (Minimum)</t>
+        </is>
+      </c>
+      <c r="C102" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" s="171" t="inlineStr">
+        <is>
+          <t>1.4.4 Resize Text</t>
+        </is>
+      </c>
+      <c r="C103" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" s="171" t="inlineStr">
+        <is>
+          <t>1.4.5 Image of Text</t>
+        </is>
+      </c>
+      <c r="C104" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" s="171" t="inlineStr">
+        <is>
+          <t>1.4.10 Reflow</t>
+        </is>
+      </c>
+      <c r="C105" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" s="171" t="inlineStr">
+        <is>
+          <t>1.4.11 Non Text Contrast</t>
+        </is>
+      </c>
+      <c r="C106" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" s="171" t="inlineStr">
+        <is>
+          <t>1.4.12 Text Spacing</t>
+        </is>
+      </c>
+      <c r="C107" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" s="171" t="inlineStr">
+        <is>
+          <t>1.4.13 Content on Hover or Focus</t>
+        </is>
+      </c>
+      <c r="C108" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="B109" s="171" t="inlineStr">
+        <is>
+          <t>2.1.1 Keyboard</t>
+        </is>
+      </c>
+      <c r="C109" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110" s="171" t="inlineStr">
+        <is>
+          <t>2.1.2 No Keyboard Trap</t>
+        </is>
+      </c>
+      <c r="C110" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111" s="171" t="inlineStr">
+        <is>
+          <t>2.1.4 Character Key Shortcut</t>
+        </is>
+      </c>
+      <c r="C111" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="B112" s="171" t="inlineStr">
+        <is>
+          <t>2.2.1 Timing Adjustable</t>
+        </is>
+      </c>
+      <c r="C112" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="B113" s="171" t="inlineStr">
+        <is>
+          <t>2.2.2 Pause, Stop, Hide</t>
+        </is>
+      </c>
+      <c r="C113" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" s="171" t="inlineStr">
+        <is>
+          <t>2.3.1 Three Flashes or Below Threshold</t>
+        </is>
+      </c>
+      <c r="C114" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="B115" s="171" t="inlineStr">
+        <is>
+          <t>2.4.1 Bypass Block</t>
+        </is>
+      </c>
+      <c r="C115" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="B116" s="171" t="inlineStr">
+        <is>
+          <t>2.4.2 Page Titled</t>
+        </is>
+      </c>
+      <c r="C116" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="B117" s="171" t="inlineStr">
+        <is>
+          <t>2.4.3 Focus Order</t>
+        </is>
+      </c>
+      <c r="C117" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="B118" s="171" t="inlineStr">
+        <is>
+          <t>2.4.4 Link Purpose (In Context)</t>
+        </is>
+      </c>
+      <c r="C118" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="B119" s="171" t="inlineStr">
+        <is>
+          <t>2.4.5 Multiple Ways</t>
+        </is>
+      </c>
+      <c r="C119" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" s="171" t="inlineStr">
+        <is>
+          <t>2.4.6 Headings and Labels</t>
+        </is>
+      </c>
+      <c r="C120" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="B121" s="171" t="inlineStr">
+        <is>
+          <t>2.4.7 Focus Visible</t>
+        </is>
+      </c>
+      <c r="C121" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="B122" s="171" t="inlineStr">
+        <is>
+          <t>2.5.1 Pointer Gestures</t>
+        </is>
+      </c>
+      <c r="C122" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="B123" s="171" t="inlineStr">
+        <is>
+          <t>2.5.2 Pointer Cancellation</t>
+        </is>
+      </c>
+      <c r="C123" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="B124" s="171" t="inlineStr">
+        <is>
+          <t>2.5.3 Label in Name</t>
+        </is>
+      </c>
+      <c r="C124" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="B125" s="171" t="inlineStr">
+        <is>
+          <t>2.5.4 Motion Actuation</t>
+        </is>
+      </c>
+      <c r="C125" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="B126" s="171" t="inlineStr">
+        <is>
+          <t>3.1.1 Language of Page</t>
+        </is>
+      </c>
+      <c r="C126" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="B127" s="171" t="inlineStr">
+        <is>
+          <t>3.1.2 Language of Parts</t>
+        </is>
+      </c>
+      <c r="C127" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="B128" s="171" t="inlineStr">
+        <is>
+          <t>3.2.1 On Focus</t>
+        </is>
+      </c>
+      <c r="C128" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" s="171" t="inlineStr">
+        <is>
+          <t>3.2.2 On Input</t>
+        </is>
+      </c>
+      <c r="C129" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" s="171" t="inlineStr">
+        <is>
+          <t>3.2.3 Consistent Navigation</t>
+        </is>
+      </c>
+      <c r="C130" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" s="171" t="inlineStr">
+        <is>
+          <t>3.2.4 Consistent Identification</t>
+        </is>
+      </c>
+      <c r="C131" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132" s="171" t="inlineStr">
+        <is>
+          <t>3.3.1 Error Identification</t>
+        </is>
+      </c>
+      <c r="C132" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" s="171" t="inlineStr">
+        <is>
+          <t>3.3.2 Label or Instructions</t>
+        </is>
+      </c>
+      <c r="C133" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134" s="171" t="inlineStr">
+        <is>
+          <t>3.3.3 Error Suggestion</t>
+        </is>
+      </c>
+      <c r="C134" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="B135" s="171" t="inlineStr">
+        <is>
+          <t>3.3.4 Error Prevention (Legal, Financial, Data)</t>
+        </is>
+      </c>
+      <c r="C135" s="171" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" s="171" t="inlineStr">
+        <is>
+          <t>4.1.1 Parsing</t>
+        </is>
+      </c>
+      <c r="C136" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="B137" s="171" t="inlineStr">
+        <is>
+          <t>4.1.2 Name, Role, Value</t>
+        </is>
+      </c>
+      <c r="C137" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138" s="171" t="inlineStr">
+        <is>
+          <t>4.1.3 Status Message</t>
+        </is>
+      </c>
+      <c r="C138" s="171" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Adding GUI Application For Control
</commit_message>
<xml_diff>
--- a/original.xlsx
+++ b/original.xlsx
@@ -24,7 +24,7 @@
     <sheet name="Notifications" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="View Statement" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="Statement Preference" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="Trying" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Data and Chart" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
@@ -1966,7 +1966,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Trying'!B82</f>
+              <f>'Data and Chart'!B82</f>
             </strRef>
           </tx>
           <spPr>
@@ -1976,12 +1976,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Trying'!$C$81:$E$81</f>
+              <f>'Data and Chart'!$C$81:$E$81</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Trying'!$C$82:$E$82</f>
+              <f>'Data and Chart'!$C$82:$E$82</f>
             </numRef>
           </val>
         </ser>
@@ -3553,7 +3553,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Trying'!C4</f>
+              <f>'Data and Chart'!C4</f>
             </strRef>
           </tx>
           <spPr>
@@ -3563,12 +3563,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Trying'!$B$5:$B$31</f>
+              <f>'Data and Chart'!$B$5:$B$31</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Trying'!$C$5:$C$31</f>
+              <f>'Data and Chart'!$C$5:$C$31</f>
             </numRef>
           </val>
         </ser>
@@ -3672,7 +3672,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Trying'!B37</f>
+              <f>'Data and Chart'!B37</f>
             </strRef>
           </tx>
           <spPr>
@@ -3682,12 +3682,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Trying'!$C$36:$F$36</f>
+              <f>'Data and Chart'!$C$36:$F$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Trying'!$C$37:$F$37</f>
+              <f>'Data and Chart'!$C$37:$F$37</f>
             </numRef>
           </val>
         </ser>
@@ -3793,7 +3793,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Trying'!B52</f>
+              <f>'Data and Chart'!B52</f>
             </strRef>
           </tx>
           <spPr>
@@ -3803,12 +3803,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Trying'!$C$51:$D$51</f>
+              <f>'Data and Chart'!$C$51:$D$51</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Trying'!$C$52:$D$52</f>
+              <f>'Data and Chart'!$C$52:$D$52</f>
             </numRef>
           </val>
         </ser>
@@ -3912,7 +3912,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Trying'!B67</f>
+              <f>'Data and Chart'!B67</f>
             </strRef>
           </tx>
           <spPr>
@@ -3922,12 +3922,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Trying'!$C$66:$I$66</f>
+              <f>'Data and Chart'!$C$66:$I$66</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Trying'!$C$67:$I$67</f>
+              <f>'Data and Chart'!$C$67:$I$67</f>
             </numRef>
           </val>
         </ser>

</xml_diff>